<commit_message>
Simplify NB01 to linear teaching flow and refresh regression datasets
</commit_message>
<xml_diff>
--- a/data/bv_fpa_regressao_nonlinear.xlsx
+++ b/data/bv_fpa_regressao_nonlinear.xlsx
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>161.0224836526987</v>
+        <v>147.5846604714236</v>
       </c>
       <c r="C39" t="n">
         <v>9.620640646055101</v>
@@ -1653,7 +1653,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>164.1009477351464</v>
+        <v>150.3752924944157</v>
       </c>
       <c r="C40" t="n">
         <v>9.865692404819532</v>
@@ -1684,7 +1684,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>160.9773869695973</v>
+        <v>146.9029309696913</v>
       </c>
       <c r="C41" t="n">
         <v>9.920692404819533</v>
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>150.5628553199429</v>
+        <v>137.2397543573069</v>
       </c>
       <c r="C42" t="n">
         <v>9.785640646055102</v>
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>144.6812567418868</v>
+        <v>130.5187793558437</v>
       </c>
       <c r="C55" t="n">
         <v>9.662232229321068</v>
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>135.3170824194263</v>
+        <v>118.6943887251082</v>
       </c>
       <c r="C56" t="n">
         <v>10.19846017549846</v>
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>124.8398033849457</v>
+        <v>104.9372488363266</v>
       </c>
       <c r="C57" t="n">
         <v>10.6106406460551</v>
@@ -2211,7 +2211,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>133.0815059421219</v>
+        <v>110.7328996911328</v>
       </c>
       <c r="C58" t="n">
         <v>10.85569240481953</v>
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>121.9422184139109</v>
+        <v>98.99442956281302</v>
       </c>
       <c r="C59" t="n">
         <v>10.91069240481954</v>
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>134.5269691413725</v>
+        <v>113.0225478581135</v>
       </c>
       <c r="C60" t="n">
         <v>10.77564064605511</v>
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>143.3037209730258</v>
+        <v>124.6236344154317</v>
       </c>
       <c r="C61" t="n">
         <v>10.47346017549846</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>160.9340916221685</v>
+        <v>145.963580174758</v>
       </c>
       <c r="C62" t="n">
         <v>10.04723222932107</v>
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>158.4110988910343</v>
+        <v>145.4050488910343</v>
       </c>
       <c r="C63" t="n">
         <v>9.555000000000001</v>
@@ -2645,7 +2645,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>126.998622274949</v>
+        <v>110.8893995203106</v>
       </c>
       <c r="C72" t="n">
         <v>10.05</v>
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>138.4906276285756</v>
+        <v>117.3294001362893</v>
       </c>
       <c r="C73" t="n">
         <v>10.65223222932107</v>

</xml_diff>